<commit_message>
Ételek bővítése, képek, mappa struktúra
</commit_message>
<xml_diff>
--- a/adatbazis/Étel lista.xlsx
+++ b/adatbazis/Étel lista.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Munka\Mutasd\mutasdmidvan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Munka\mutasd2\mutasdmidvan\adatbazis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B049F035-9206-44C3-8022-E1F3226600CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6D79F7-4CBB-455D-965C-7DB3CEDFF430}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{7882C499-AA6B-4843-9FCE-FD484EF25E37}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Reggeli</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Gyömbéres sárgarépakrémleves</t>
+  </si>
+  <si>
+    <t>Sorszám</t>
+  </si>
+  <si>
+    <t>Kép?</t>
   </si>
 </sst>
 </file>
@@ -158,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +180,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -205,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -219,6 +231,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -533,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1410A1-52C3-4A35-AF37-7E2E00B70184}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +573,7 @@
     <col min="9" max="9" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -581,8 +602,14 @@
       <c r="J1" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -595,8 +622,12 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="6"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="8">
+        <v>1</v>
+      </c>
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
@@ -609,8 +640,12 @@
       <c r="H3" s="6"/>
       <c r="I3" s="1"/>
       <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="8">
+        <v>2</v>
+      </c>
+      <c r="L3" s="9"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -623,8 +658,12 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="8">
+        <v>3</v>
+      </c>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -637,8 +676,12 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="8">
+        <v>4</v>
+      </c>
+      <c r="L5" s="8"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -651,8 +694,12 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="8">
+        <v>5</v>
+      </c>
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -665,8 +712,12 @@
       <c r="H7" s="1"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="8">
+        <v>6</v>
+      </c>
+      <c r="L7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -679,8 +730,12 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="8">
+        <v>7</v>
+      </c>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -693,8 +748,12 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="8">
+        <v>8</v>
+      </c>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -707,8 +766,12 @@
       <c r="H10" s="1"/>
       <c r="I10" s="6"/>
       <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="8">
+        <v>9</v>
+      </c>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -721,8 +784,12 @@
       <c r="H11" s="6"/>
       <c r="I11" s="1"/>
       <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="8">
+        <v>10</v>
+      </c>
+      <c r="L11" s="8"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -735,8 +802,12 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="8">
+        <v>11</v>
+      </c>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
@@ -749,8 +820,12 @@
       <c r="H13" s="1"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="8">
+        <v>12</v>
+      </c>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -763,8 +838,12 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="8">
+        <v>13</v>
+      </c>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
@@ -777,8 +856,12 @@
       <c r="H15" s="6"/>
       <c r="I15" s="1"/>
       <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="8">
+        <v>14</v>
+      </c>
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -791,8 +874,12 @@
       <c r="H16" s="1"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="8">
+        <v>15</v>
+      </c>
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -805,8 +892,12 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="8">
+        <v>16</v>
+      </c>
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
@@ -819,8 +910,12 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="6"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="8">
+        <v>17</v>
+      </c>
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
@@ -833,8 +928,12 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="8">
+        <v>18</v>
+      </c>
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>11</v>
       </c>
@@ -847,8 +946,12 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="6"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="8">
+        <v>19</v>
+      </c>
+      <c r="L20" s="8"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
@@ -861,8 +964,12 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="8">
+        <v>20</v>
+      </c>
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
@@ -875,8 +982,12 @@
       <c r="H22" s="6"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="8">
+        <v>21</v>
+      </c>
+      <c r="L22" s="8"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -889,8 +1000,12 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="8">
+        <v>22</v>
+      </c>
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
@@ -903,8 +1018,12 @@
       <c r="H24" s="6"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="8">
+        <v>23</v>
+      </c>
+      <c r="L24" s="8"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>27</v>
       </c>
@@ -917,8 +1036,12 @@
       <c r="H25" s="1"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="8">
+        <v>24</v>
+      </c>
+      <c r="L25" s="9"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -931,8 +1054,12 @@
       <c r="H26" s="1"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="8">
+        <v>25</v>
+      </c>
+      <c r="L26" s="9"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>16</v>
       </c>
@@ -945,8 +1072,12 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="6"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" s="8">
+        <v>26</v>
+      </c>
+      <c r="L27" s="8"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
@@ -959,8 +1090,12 @@
       <c r="H28" s="1"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="8">
+        <v>27</v>
+      </c>
+      <c r="L28" s="8"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
@@ -973,8 +1108,12 @@
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" s="8">
+        <v>28</v>
+      </c>
+      <c r="L29" s="9"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>37</v>
       </c>
@@ -987,8 +1126,12 @@
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" s="8">
+        <v>29</v>
+      </c>
+      <c r="L30" s="8"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>38</v>
       </c>
@@ -1001,8 +1144,12 @@
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" s="8">
+        <v>30</v>
+      </c>
+      <c r="L31" s="9"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
htdocs mappába dolgozás, htaccess megírása, mutasd.php szintaktika elkészítése
</commit_message>
<xml_diff>
--- a/adatbazis/Étel lista.xlsx
+++ b/adatbazis/Étel lista.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Munka\mutasd2\mutasdmidvan\adatbazis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Munka\13c-eszter\mutasdmidvan\adatbazis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6D79F7-4CBB-455D-965C-7DB3CEDFF430}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD1232D-4969-4439-B06C-A5C4BCFCC695}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{7882C499-AA6B-4843-9FCE-FD484EF25E37}"/>
   </bookViews>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1410A1-52C3-4A35-AF37-7E2E00B70184}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +679,7 @@
       <c r="K5" s="8">
         <v>4</v>
       </c>
-      <c r="L5" s="8"/>
+      <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -715,7 +715,7 @@
       <c r="K7" s="8">
         <v>6</v>
       </c>
-      <c r="L7" s="8"/>
+      <c r="L7" s="9"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -805,7 +805,7 @@
       <c r="K12" s="8">
         <v>11</v>
       </c>
-      <c r="L12" s="8"/>
+      <c r="L12" s="9"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -859,7 +859,7 @@
       <c r="K15" s="8">
         <v>14</v>
       </c>
-      <c r="L15" s="8"/>
+      <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -931,7 +931,7 @@
       <c r="K19" s="8">
         <v>18</v>
       </c>
-      <c r="L19" s="8"/>
+      <c r="L19" s="9"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -949,7 +949,7 @@
       <c r="K20" s="8">
         <v>19</v>
       </c>
-      <c r="L20" s="8"/>
+      <c r="L20" s="9"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -967,7 +967,7 @@
       <c r="K21" s="8">
         <v>20</v>
       </c>
-      <c r="L21" s="8"/>
+      <c r="L21" s="9"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -985,7 +985,7 @@
       <c r="K22" s="8">
         <v>21</v>
       </c>
-      <c r="L22" s="8"/>
+      <c r="L22" s="9"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -1003,7 +1003,7 @@
       <c r="K23" s="8">
         <v>22</v>
       </c>
-      <c r="L23" s="8"/>
+      <c r="L23" s="9"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -1021,7 +1021,7 @@
       <c r="K24" s="8">
         <v>23</v>
       </c>
-      <c r="L24" s="8"/>
+      <c r="L24" s="9"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
@@ -1093,7 +1093,7 @@
       <c r="K28" s="8">
         <v>27</v>
       </c>
-      <c r="L28" s="8"/>
+      <c r="L28" s="9"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
@@ -1129,7 +1129,7 @@
       <c r="K30" s="8">
         <v>29</v>
       </c>
-      <c r="L30" s="8"/>
+      <c r="L30" s="9"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">

</xml_diff>

<commit_message>
0317, adatbázis bővítése, javítása, regisztráció hibátlan működése, bejelentkezés hiba javítások
</commit_message>
<xml_diff>
--- a/adatbazis/Étel lista.xlsx
+++ b/adatbazis/Étel lista.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Munka\13c-eszter\mutasdmidvan\adatbazis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\13eszter\mutasdmidvan\adatbazis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD1232D-4969-4439-B06C-A5C4BCFCC695}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE83312B-6CE8-4075-9CAD-690830AB0CA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{7882C499-AA6B-4843-9FCE-FD484EF25E37}"/>
   </bookViews>
@@ -154,7 +154,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,8 +163,16 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +194,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -217,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -240,6 +254,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -554,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1410A1-52C3-4A35-AF37-7E2E00B70184}">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +589,7 @@
     <col min="9" max="9" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -608,8 +624,9 @@
       <c r="L1" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -626,8 +643,9 @@
         <v>1</v>
       </c>
       <c r="L2" s="9"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="10"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
@@ -644,8 +662,9 @@
         <v>2</v>
       </c>
       <c r="L3" s="9"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="10"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -662,8 +681,9 @@
         <v>3</v>
       </c>
       <c r="L4" s="9"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="11"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -680,8 +700,9 @@
         <v>4</v>
       </c>
       <c r="L5" s="9"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -698,8 +719,9 @@
         <v>5</v>
       </c>
       <c r="L6" s="9"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -716,8 +738,9 @@
         <v>6</v>
       </c>
       <c r="L7" s="9"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -734,8 +757,9 @@
         <v>7</v>
       </c>
       <c r="L8" s="9"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -752,8 +776,9 @@
         <v>8</v>
       </c>
       <c r="L9" s="9"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -770,8 +795,9 @@
         <v>9</v>
       </c>
       <c r="L10" s="9"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -788,8 +814,9 @@
         <v>10</v>
       </c>
       <c r="L11" s="8"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -806,8 +833,9 @@
         <v>11</v>
       </c>
       <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
@@ -824,8 +852,9 @@
         <v>12</v>
       </c>
       <c r="L13" s="9"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -842,8 +871,9 @@
         <v>13</v>
       </c>
       <c r="L14" s="9"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
@@ -860,8 +890,9 @@
         <v>14</v>
       </c>
       <c r="L15" s="9"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -878,8 +909,9 @@
         <v>15</v>
       </c>
       <c r="L16" s="9"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -896,8 +928,9 @@
         <v>16</v>
       </c>
       <c r="L17" s="9"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
@@ -914,8 +947,9 @@
         <v>17</v>
       </c>
       <c r="L18" s="9"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
@@ -932,8 +966,9 @@
         <v>18</v>
       </c>
       <c r="L19" s="9"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>11</v>
       </c>
@@ -950,8 +985,9 @@
         <v>19</v>
       </c>
       <c r="L20" s="9"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
@@ -968,8 +1004,9 @@
         <v>20</v>
       </c>
       <c r="L21" s="9"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
@@ -986,8 +1023,9 @@
         <v>21</v>
       </c>
       <c r="L22" s="9"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -1004,8 +1042,9 @@
         <v>22</v>
       </c>
       <c r="L23" s="9"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
@@ -1022,8 +1061,9 @@
         <v>23</v>
       </c>
       <c r="L24" s="9"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>27</v>
       </c>
@@ -1040,8 +1080,9 @@
         <v>24</v>
       </c>
       <c r="L25" s="9"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -1058,8 +1099,9 @@
         <v>25</v>
       </c>
       <c r="L26" s="9"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" s="10"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>16</v>
       </c>
@@ -1076,8 +1118,9 @@
         <v>26</v>
       </c>
       <c r="L27" s="8"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
@@ -1094,8 +1137,9 @@
         <v>27</v>
       </c>
       <c r="L28" s="9"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28" s="1"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
@@ -1112,8 +1156,9 @@
         <v>28</v>
       </c>
       <c r="L29" s="9"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>37</v>
       </c>
@@ -1130,8 +1175,9 @@
         <v>29</v>
       </c>
       <c r="L30" s="9"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>38</v>
       </c>
@@ -1148,8 +1194,9 @@
         <v>30</v>
       </c>
       <c r="L31" s="9"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
minden étel fent van adatbázisba, hozzávalók hozzárendelése.
</commit_message>
<xml_diff>
--- a/adatbazis/Étel lista.xlsx
+++ b/adatbazis/Étel lista.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\13eszter\mutasdmidvan\adatbazis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE83312B-6CE8-4075-9CAD-690830AB0CA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD9B60E-F24F-484D-AAE4-0C02A55EE16D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{7882C499-AA6B-4843-9FCE-FD484EF25E37}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Reggeli</t>
   </si>
@@ -148,6 +148,15 @@
   </si>
   <si>
     <t>Kép?</t>
+  </si>
+  <si>
+    <t>!!KÉP</t>
+  </si>
+  <si>
+    <t>Adatbázisba</t>
+  </si>
+  <si>
+    <t>Hozzávalóval</t>
   </si>
 </sst>
 </file>
@@ -172,7 +181,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,6 +209,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -233,18 +248,9 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -254,8 +260,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -570,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1410A1-52C3-4A35-AF37-7E2E00B70184}">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,9 +612,12 @@
     <col min="7" max="7" width="17.7109375" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="5"/>
+    <col min="15" max="15" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -606,607 +634,677 @@
       <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="6"/>
+      <c r="O1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="8">
+      <c r="B2" s="7"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="3">
         <v>1</v>
       </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="10"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L2" s="4"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="8">
+      <c r="B3" s="3"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="3">
         <v>2</v>
       </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="10"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L3" s="4"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="9"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="8">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="3">
         <v>3</v>
       </c>
-      <c r="L4" s="9"/>
-      <c r="M4" s="11"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L4" s="4"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="8">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3">
         <v>4</v>
       </c>
-      <c r="L5" s="9"/>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L5" s="4"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="8">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="3">
         <v>5</v>
       </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L6" s="4"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="8">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="3">
         <v>6</v>
       </c>
-      <c r="L7" s="9"/>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L7" s="4"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="8">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="3">
         <v>7</v>
       </c>
-      <c r="L8" s="9"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L8" s="4"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="8">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="3">
         <v>8</v>
       </c>
-      <c r="L9" s="9"/>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L9" s="4"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="8">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3">
         <v>9</v>
       </c>
-      <c r="L10" s="9"/>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L10" s="4"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="8">
+      <c r="B11" s="7"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="3">
         <v>10</v>
       </c>
-      <c r="L11" s="8"/>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L11" s="4"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="8">
+      <c r="B12" s="3"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="3">
         <v>11</v>
       </c>
-      <c r="L12" s="9"/>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L12" s="4"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="8">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="3">
         <v>12</v>
       </c>
-      <c r="L13" s="9"/>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L13" s="4"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="8">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="3">
         <v>13</v>
       </c>
-      <c r="L14" s="9"/>
-      <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L14" s="4"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="8">
+      <c r="B15" s="7"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="3">
         <v>14</v>
       </c>
-      <c r="L15" s="9"/>
-      <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L15" s="4"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="8">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="3">
         <v>15</v>
       </c>
-      <c r="L16" s="9"/>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L16" s="4"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="8">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3">
         <v>16</v>
       </c>
-      <c r="L17" s="9"/>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L17" s="4"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="8">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="3">
         <v>17</v>
       </c>
-      <c r="L18" s="9"/>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L18" s="4"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="8">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3">
         <v>18</v>
       </c>
-      <c r="L19" s="9"/>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L19" s="4"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="8">
+      <c r="B20" s="3"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="3">
         <v>19</v>
       </c>
-      <c r="L20" s="9"/>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L20" s="4"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="3"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="8">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="3">
         <v>20</v>
       </c>
-      <c r="L21" s="9"/>
-      <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L21" s="4"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="8">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3">
         <v>21</v>
       </c>
-      <c r="L22" s="9"/>
-      <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L22" s="4"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="8">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="3">
         <v>22</v>
       </c>
-      <c r="L23" s="9"/>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L23" s="4"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="8">
+      <c r="B24" s="7"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3">
         <v>23</v>
       </c>
-      <c r="L24" s="9"/>
-      <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L24" s="4"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="8">
+      <c r="B25" s="3"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="3">
         <v>24</v>
       </c>
-      <c r="L25" s="9"/>
-      <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L25" s="4"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="3"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="8">
+      <c r="B26" s="3"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="3">
         <v>25</v>
       </c>
-      <c r="L26" s="9"/>
-      <c r="M26" s="10"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L26" s="4"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="9"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="8">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="3">
         <v>26</v>
       </c>
-      <c r="L27" s="8"/>
-      <c r="M27" s="1"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L27" s="4"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="8">
+      <c r="B28" s="3"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="3">
         <v>27</v>
       </c>
-      <c r="L28" s="9"/>
-      <c r="M28" s="1"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L28" s="4"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="8">
+      <c r="B29" s="7"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="3">
         <v>28</v>
       </c>
-      <c r="L29" s="9"/>
-      <c r="M29" s="1"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L29" s="4"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="3"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="8">
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="3">
         <v>29</v>
       </c>
-      <c r="L30" s="9"/>
-      <c r="M30" s="1"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L30" s="4"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="3"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="8">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="3">
         <v>30</v>
       </c>
-      <c r="L31" s="9"/>
-      <c r="M31" s="1"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="3"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
+      <c r="A33" s="1"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
+      <c r="A34" s="1"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
+      <c r="A35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
hozzávalók feltöltése, vega, vegán ételek kiválasztása már kész az adatbázisba
</commit_message>
<xml_diff>
--- a/adatbazis/Étel lista.xlsx
+++ b/adatbazis/Étel lista.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\13eszter\mutasdmidvan\adatbazis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7E52F5-CEEE-4D40-88E7-08C4E87A163A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68645F65-97AA-46D0-B370-0F1C0D5D45DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{7882C499-AA6B-4843-9FCE-FD484EF25E37}"/>
   </bookViews>
@@ -598,7 +598,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,7 +784,7 @@
       <c r="L7" s="4"/>
       <c r="M7" s="9"/>
       <c r="N7" s="6"/>
-      <c r="O7" s="3"/>
+      <c r="O7" s="9"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">

</xml_diff>